<commit_message>
Changed reset scholarships data.
</commit_message>
<xml_diff>
--- a/tests/data/scholarships.xlsx
+++ b/tests/data/scholarships.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +504,21 @@
           <t>HS Percentile</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Group One</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Group Two</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Group Three</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -511,98 +526,85 @@
           <t>Test One</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C2" t="n">
-        <v>8000</v>
-      </c>
-      <c r="D2" t="n">
-        <v>315</v>
-      </c>
-      <c r="E2" t="n">
-        <v>26</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>315</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>All</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>25</v>
-      </c>
-      <c r="H2" t="n">
-        <v>27</v>
-      </c>
-      <c r="I2" t="n">
-        <v>26</v>
-      </c>
-      <c r="J2" t="n">
-        <v>600</v>
-      </c>
-      <c r="K2" t="n">
-        <v>400</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M2" t="n">
-        <v>4</v>
-      </c>
-      <c r="N2" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Test Two</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>10000</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>330</v>
-      </c>
-      <c r="E3" t="n">
-        <v>30</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>32</v>
-      </c>
-      <c r="H3" t="n">
-        <v>28</v>
-      </c>
-      <c r="I3" t="n">
-        <v>30</v>
-      </c>
-      <c r="J3" t="n">
-        <v>700</v>
-      </c>
-      <c r="K3" t="n">
-        <v>620</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1320</v>
-      </c>
-      <c r="M3" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="N3" t="n">
-        <v>95</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>['ACT Math', 'SAT Math']</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>['ACT Composite', 'SAT Combined']</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fully updated create; see NOTE at to_excel
</commit_message>
<xml_diff>
--- a/tests/data/scholarships.xlsx
+++ b/tests/data/scholarships.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,84 +526,127 @@
           <t>Test One</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>315</v>
+      </c>
+      <c r="E2" t="n">
+        <v>26</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>25</v>
+      </c>
+      <c r="H2" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2" t="n">
+        <v>26</v>
+      </c>
+      <c r="J2" t="n">
+        <v>600</v>
+      </c>
+      <c r="K2" t="n">
+        <v>400</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="M2" t="n">
+        <v>4</v>
+      </c>
+      <c r="N2" t="n">
+        <v>96</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>['ACT Math', 'SAT Math']</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>['ACT Composite', 'SAT Combined']</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>New Scholarship</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>1000</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>8000</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>315</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>600</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
+      <c r="D3" t="n">
+        <v>210</v>
+      </c>
+      <c r="E3" t="n">
+        <v>23</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Computer Science and Engineering</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>23</v>
+      </c>
+      <c r="H3" t="n">
+        <v>19</v>
+      </c>
+      <c r="I3" t="n">
+        <v>21</v>
+      </c>
+      <c r="J3" t="n">
+        <v>530</v>
+      </c>
+      <c r="K3" t="n">
+        <v>370</v>
+      </c>
+      <c r="L3" t="n">
+        <v>900</v>
+      </c>
+      <c r="M3" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="N3" t="n">
+        <v>75</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>['ACT Composite', 'SAT Combined']</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
         <is>
           <t>['ACT Math', 'SAT Math']</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>['ACT Composite', 'SAT Combined']</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>[]</t>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>['GPA', 'HS Percentile']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated scholarships to match Austin's changes
</commit_message>
<xml_diff>
--- a/tests/data/scholarships.xlsx
+++ b/tests/data/scholarships.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,22 +451,57 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>RAI</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Admit Score</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Major</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>ACT</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>SAT</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>ACT Math</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ACT English</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ACT Composite</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SAT Math</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>SAT Reading</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>SAT Combined</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>GPA</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>HS Percentile</t>
         </is>
       </c>
     </row>
@@ -482,50 +517,92 @@
       <c r="C2" t="n">
         <v>8000</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
+      <c r="D2" t="n">
+        <v>315</v>
       </c>
       <c r="E2" t="n">
         <v>26</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>25</v>
+      </c>
+      <c r="H2" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2" t="n">
+        <v>26</v>
+      </c>
+      <c r="J2" t="n">
+        <v>600</v>
+      </c>
+      <c r="K2" t="n">
+        <v>400</v>
+      </c>
+      <c r="L2" t="n">
         <v>1000</v>
       </c>
-      <c r="G2" t="n">
+      <c r="M2" t="n">
         <v>4</v>
+      </c>
+      <c r="N2" t="n">
+        <v>96</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cool Kids Club</t>
+          <t>Test Two</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>50</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>11111111</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Computer Science and Engineering</t>
-        </is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>330</v>
       </c>
       <c r="E3" t="n">
-        <v>36</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1600</v>
+        <v>30</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
       </c>
       <c r="G3" t="n">
-        <v>4.95</v>
+        <v>32</v>
+      </c>
+      <c r="H3" t="n">
+        <v>28</v>
+      </c>
+      <c r="I3" t="n">
+        <v>30</v>
+      </c>
+      <c r="J3" t="n">
+        <v>700</v>
+      </c>
+      <c r="K3" t="n">
+        <v>620</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1320</v>
+      </c>
+      <c r="M3" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="N3" t="n">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>